<commit_message>
SASS + HEAD HTML
</commit_message>
<xml_diff>
--- a/roadmap.xlsx
+++ b/roadmap.xlsx
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1021,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L18" s="3"/>

</xml_diff>